<commit_message>
Made changs for Localisation and added test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebFeatureData.xlsx
+++ b/src/test/resources/testdata/WebFeatureData.xlsx
@@ -3,14 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="TestCaseData" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="default" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="en-us" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="es" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7miXA/nhthidKApIU0siLRh1NOVGAg=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
   <si>
     <t>testCaseId</t>
   </si>
@@ -30,6 +37,21 @@
     <t>featureFile</t>
   </si>
   <si>
+    <t>rememberMe</t>
+  </si>
+  <si>
+    <t>useToken</t>
+  </si>
+  <si>
+    <t>signInButton</t>
+  </si>
+  <si>
+    <t>forgotLink</t>
+  </si>
+  <si>
+    <t>signUp</t>
+  </si>
+  <si>
     <t>accountNumber</t>
   </si>
   <si>
@@ -39,40 +61,76 @@
     <t>userName</t>
   </si>
   <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
     <t>JPMC-1</t>
   </si>
   <si>
-    <t>arunsubramanian.veerabahu@photoninfotech.net</t>
-  </si>
-  <si>
-    <t>JPMC1</t>
-  </si>
-  <si>
-    <t>danhams</t>
-  </si>
-  <si>
-    <t>Verify the links in jpmc rewards page</t>
-  </si>
-  <si>
-    <t>JpmcRewardsPage</t>
+    <t>kirankumar.baskar@photoninfotech.net</t>
+  </si>
+  <si>
+    <t>Kiran Kumar V</t>
+  </si>
+  <si>
+    <t>Verify login with invalid credentials</t>
+  </si>
+  <si>
+    <t>JPMCSignin</t>
+  </si>
+  <si>
+    <t>Recuérdame</t>
+  </si>
+  <si>
+    <t>Usa token</t>
+  </si>
+  <si>
+    <t>Remember me</t>
+  </si>
+  <si>
+    <t>Iniciar sesión</t>
+  </si>
+  <si>
+    <t>Use token</t>
+  </si>
+  <si>
+    <t>¿Olvidaste tu nombre de usuario o contraseña?</t>
+  </si>
+  <si>
+    <t>Sign in</t>
+  </si>
+  <si>
+    <t>¿No estás inscrito? Regístrate ahora.</t>
+  </si>
+  <si>
+    <t>Forgot username/password?</t>
+  </si>
+  <si>
+    <t>Not Enrolled? Sign Up Now.</t>
   </si>
   <si>
     <t>JPMC-2</t>
   </si>
   <si>
-    <t>raghu.krishnan@photoninfotech.net</t>
-  </si>
-  <si>
-    <t>JPMC-44</t>
-  </si>
-  <si>
-    <t>Verify the signup in jpmc rewards page</t>
+    <t>Raghu K</t>
+  </si>
+  <si>
+    <t>Verify signup in JPMC rewards page</t>
   </si>
   <si>
     <t>danharms2</t>
   </si>
   <si>
-    <t>JPMC-45</t>
+    <t>Unable to register your account as given account number does not matches</t>
+  </si>
+  <si>
+    <t>No se puede registrar su cuenta ya que el número de cuenta dado no coincide</t>
+  </si>
+  <si>
+    <t>JPMC-7</t>
+  </si>
+  <si>
+    <t>JPMC-9</t>
   </si>
 </sst>
 </file>
@@ -80,7 +138,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -96,21 +154,27 @@
     </font>
     <font>
       <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
-    <font>
-      <sz val="11.0"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -143,23 +207,17 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -170,6 +228,14 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -377,11 +443,21 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.43" collapsed="false"/>
-    <col min="2" max="5" customWidth="true" width="36.14" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="18.29" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.57" collapsed="false"/>
-    <col min="8" max="9" customWidth="true" width="14.43" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.86" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.43" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.86" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.43" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.57" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.43" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="24.71" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.14" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.57" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.57" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.43" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="63.43" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -391,7 +467,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -412,63 +488,99 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
+      <c r="A2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C2" s="5"/>
       <c r="D2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="8">
         <v>1.2345678901234E13</v>
       </c>
-      <c r="H3" s="1">
+      <c r="M3" s="8">
         <v>9.89898976E8</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>19</v>
+      <c r="N3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="8"/>
-    </row>
+    <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>
@@ -1462,8 +1574,312 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.86" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.43" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.86" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.43" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.57" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.43" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="24.71" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.14" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.57" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.57" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.43" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="63.43" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="8">
+        <v>1.2345678901234E13</v>
+      </c>
+      <c r="M3" s="8">
+        <v>9.89898976E8</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.86" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.43" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.86" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.43" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.57" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="40.43" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="31.86" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.57" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.57" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.43" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="65.71" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="8">
+        <v>1.2345678901234E13</v>
+      </c>
+      <c r="M3" s="8">
+        <v>9.89898976E8</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added JPMC UAT team demo script
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebFeatureData.xlsx
+++ b/src/test/resources/testdata/WebFeatureData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="45">
   <si>
     <t>testCaseId</t>
   </si>
@@ -79,42 +79,39 @@
     <t>JPMCSignin</t>
   </si>
   <si>
+    <t>Remember me</t>
+  </si>
+  <si>
+    <t>Use token</t>
+  </si>
+  <si>
     <t>Recuérdame</t>
   </si>
   <si>
     <t>Usa token</t>
   </si>
   <si>
-    <t>Remember me</t>
+    <t>Sign in</t>
   </si>
   <si>
     <t>Iniciar sesión</t>
   </si>
   <si>
-    <t>Use token</t>
+    <t>Forgot username/password?</t>
   </si>
   <si>
     <t>¿Olvidaste tu nombre de usuario o contraseña?</t>
   </si>
   <si>
-    <t>Sign in</t>
+    <t>Not Enrolled? Sign Up Now.</t>
   </si>
   <si>
     <t>¿No estás inscrito? Regístrate ahora.</t>
   </si>
   <si>
-    <t>Forgot username/password?</t>
-  </si>
-  <si>
-    <t>Not Enrolled? Sign Up Now.</t>
-  </si>
-  <si>
     <t>JPMC-2</t>
   </si>
   <si>
-    <t>Raghu K</t>
-  </si>
-  <si>
     <t>Verify signup in JPMC rewards page</t>
   </si>
   <si>
@@ -124,13 +121,37 @@
     <t>Unable to register your account as given account number does not matches</t>
   </si>
   <si>
+    <t>JPMC-14</t>
+  </si>
+  <si>
+    <t>Home Page Visual Validation</t>
+  </si>
+  <si>
     <t>No se puede registrar su cuenta ya que el número de cuenta dado no coincide</t>
   </si>
   <si>
-    <t>JPMC-7</t>
-  </si>
-  <si>
-    <t>JPMC-9</t>
+    <t>JPMC-15</t>
+  </si>
+  <si>
+    <t>Page Load Performance Validation</t>
+  </si>
+  <si>
+    <t>JPMC-16</t>
+  </si>
+  <si>
+    <t>Find a credit card for Personal Rewards Cash Back Balance Transfer</t>
+  </si>
+  <si>
+    <t>Functional validation of Find a Card</t>
+  </si>
+  <si>
+    <t>JPMC-17</t>
+  </si>
+  <si>
+    <t>Find a credit card for Business Rewards Cash Back</t>
+  </si>
+  <si>
+    <t>JPMC-20</t>
   </si>
 </sst>
 </file>
@@ -138,7 +159,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -155,11 +176,6 @@
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -203,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -212,10 +228,6 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -443,21 +455,21 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="8.86" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="32.43" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.86" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.43" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="9.57" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.43" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="24.71" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="24.14" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.57" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.57" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.43" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="63.43" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="43.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="8.86" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="16.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="58.0" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="30.43" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="13.43" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="9.57" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="11.43" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="24.71" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="24.14" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="15.57" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.57" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.43" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="63.43" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -515,7 +527,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -525,19 +537,19 @@
         <v>19</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -552,11 +564,11 @@
         <v>16</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>19</v>
@@ -566,23 +578,127 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="8">
+      <c r="L3" s="6">
         <v>1.2345678901234E13</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="6">
         <v>9.89898976E8</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="5" t="s">
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1"/>
     <row r="10" ht="15.75" customHeight="1"/>
@@ -1589,21 +1705,21 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="8.86" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="32.43" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.86" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.43" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="9.57" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.43" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="24.71" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="24.14" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.57" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.57" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.43" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="63.43" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="43.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="8.86" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="16.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="58.0" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="30.43" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="13.43" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="9.57" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="11.43" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="24.71" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="24.14" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="15.57" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.57" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.43" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="63.43" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1661,7 +1777,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1671,19 +1787,19 @@
         <v>19</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -1694,17 +1810,15 @@
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>19</v>
@@ -1714,18 +1828,128 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="8">
+      <c r="L3" s="6">
         <v>1.2345678901234E13</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="6">
         <v>9.89898976E8</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="5" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1742,21 +1966,21 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="8.86" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="32.43" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.86" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.43" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="9.57" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="40.43" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="31.86" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.57" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.57" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.43" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="65.71" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="10.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="43.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="8.86" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="16.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="58.0" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="30.43" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="13.43" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="9.57" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="40.43" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="31.86" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="15.57" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="10.57" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="10.43" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="65.71" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1814,7 +2038,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1824,19 +2048,19 @@
         <v>19</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -1847,17 +2071,15 @@
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>19</v>
@@ -1867,18 +2089,126 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="8">
+      <c r="L3" s="6">
         <v>1.2345678901234E13</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="6">
         <v>9.89898976E8</v>
       </c>
-      <c r="N3" s="8" t="s">
-        <v>33</v>
+      <c r="N3" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="O3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Jira Integration issue fix
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebFeatureData.xlsx
+++ b/src/test/resources/testdata/WebFeatureData.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7miXA/nhthidKApIU0siLRh1NOVGAg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mhV7SK4lq3VOrSWVmQGtJtI1ub1iQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="50">
   <si>
     <t>testCaseId</t>
   </si>
@@ -64,12 +64,51 @@
     <t>errorMessage</t>
   </si>
   <si>
+    <t>DEMO-1</t>
+  </si>
+  <si>
+    <t>kirankumar.baskar@photoninfotech.net</t>
+  </si>
+  <si>
+    <t>Kiran Kumar</t>
+  </si>
+  <si>
+    <t>Find a credit card for Personal Rewards Cash Back Balance Transfer</t>
+  </si>
+  <si>
+    <t>FindaCard</t>
+  </si>
+  <si>
+    <t>Remember me</t>
+  </si>
+  <si>
+    <t>Use token</t>
+  </si>
+  <si>
+    <t>Sign in</t>
+  </si>
+  <si>
+    <t>Forgot username/password?</t>
+  </si>
+  <si>
+    <t>Not Enrolled? Sign Up Now.</t>
+  </si>
+  <si>
+    <t>DEMO-2</t>
+  </si>
+  <si>
+    <t>Find a credit card for Business Rewards Cash Back</t>
+  </si>
+  <si>
+    <t>danharms2</t>
+  </si>
+  <si>
+    <t>Unable to register your account as given account number does not matches</t>
+  </si>
+  <si>
     <t>JPMC-1</t>
   </si>
   <si>
-    <t>kirankumar.baskar@photoninfotech.net</t>
-  </si>
-  <si>
     <t>Kiran Kumar V</t>
   </si>
   <si>
@@ -79,10 +118,34 @@
     <t>JPMCSignin</t>
   </si>
   <si>
-    <t>Remember me</t>
-  </si>
-  <si>
-    <t>Use token</t>
+    <t>JPMC-2</t>
+  </si>
+  <si>
+    <t>Verify signup in JPMC rewards page</t>
+  </si>
+  <si>
+    <t>JPMC-14</t>
+  </si>
+  <si>
+    <t>Home Page Visual Validation</t>
+  </si>
+  <si>
+    <t>JPMC-15</t>
+  </si>
+  <si>
+    <t>Page Load Performance Validation</t>
+  </si>
+  <si>
+    <t>JPMC-16</t>
+  </si>
+  <si>
+    <t>JPMC-20</t>
+  </si>
+  <si>
+    <t>Functional validation of Find a Card</t>
+  </si>
+  <si>
+    <t>JPMC-17</t>
   </si>
   <si>
     <t>Recuérdame</t>
@@ -91,67 +154,19 @@
     <t>Usa token</t>
   </si>
   <si>
-    <t>Sign in</t>
-  </si>
-  <si>
     <t>Iniciar sesión</t>
   </si>
   <si>
-    <t>Forgot username/password?</t>
-  </si>
-  <si>
     <t>¿Olvidaste tu nombre de usuario o contraseña?</t>
   </si>
   <si>
-    <t>Not Enrolled? Sign Up Now.</t>
-  </si>
-  <si>
     <t>¿No estás inscrito? Regístrate ahora.</t>
   </si>
   <si>
-    <t>JPMC-2</t>
-  </si>
-  <si>
-    <t>Verify signup in JPMC rewards page</t>
-  </si>
-  <si>
-    <t>danharms2</t>
-  </si>
-  <si>
-    <t>Unable to register your account as given account number does not matches</t>
-  </si>
-  <si>
-    <t>JPMC-14</t>
-  </si>
-  <si>
-    <t>Home Page Visual Validation</t>
-  </si>
-  <si>
     <t>No se puede registrar su cuenta ya que el número de cuenta dado no coincide</t>
   </si>
   <si>
-    <t>JPMC-15</t>
-  </si>
-  <si>
-    <t>Page Load Performance Validation</t>
-  </si>
-  <si>
-    <t>JPMC-16</t>
-  </si>
-  <si>
-    <t>Find a credit card for Personal Rewards Cash Back Balance Transfer</t>
-  </si>
-  <si>
-    <t>Functional validation of Find a Card</t>
-  </si>
-  <si>
-    <t>JPMC-17</t>
-  </si>
-  <si>
-    <t>Find a credit card for Business Rewards Cash Back</t>
-  </si>
-  <si>
-    <t>JPMC-20</t>
+    <t>DEMO-3</t>
   </si>
 </sst>
 </file>
@@ -219,18 +234,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -526,7 +544,9 @@
       <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
@@ -543,13 +563,13 @@
         <v>21</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -558,7 +578,7 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>16</v>
@@ -568,7 +588,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>19</v>
@@ -585,120 +605,16 @@
         <v>9.89898976E8</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-    </row>
+    <row r="4" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1"/>
+    <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1"/>
     <row r="10" ht="15.75" customHeight="1"/>
@@ -1686,10 +1602,6 @@
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
     <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1770,21 +1682,21 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
+      <c r="A2" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>19</v>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>20</v>
@@ -1793,13 +1705,13 @@
         <v>21</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -1807,21 +1719,21 @@
       <c r="O2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>30</v>
+      <c r="A3" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
+      <c r="D3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -1835,28 +1747,28 @@
         <v>9.89898976E8</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>34</v>
+      <c r="A4" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
+      <c r="D4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1869,21 +1781,21 @@
       <c r="O4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
+      <c r="F5" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -1896,20 +1808,20 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>40</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>41</v>
@@ -1925,18 +1837,18 @@
       <c r="O6" s="5"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
+      <c r="D7" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>41</v>
@@ -2031,36 +1943,36 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
+      <c r="A2" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>19</v>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -2068,21 +1980,21 @@
       <c r="O2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>30</v>
+      <c r="A3" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
+      <c r="D3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -2096,28 +2008,28 @@
         <v>9.89898976E8</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>34</v>
+      <c r="A4" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
+      <c r="D4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -2130,21 +2042,21 @@
       <c r="O4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
+      <c r="F5" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -2157,18 +2069,18 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
+      <c r="D6" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>41</v>
@@ -2184,18 +2096,18 @@
       <c r="O6" s="5"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
+      <c r="D7" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>41</v>

</xml_diff>